<commit_message>
Added Whole features of View and manage staff including adding, update, delete staff
</commit_message>
<xml_diff>
--- a/data/Auth_Data.xlsx
+++ b/data/Auth_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\IdeaProjects\SC2002_Project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{6C86D8D1-F53D-4A46-A84B-73E16564535E}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr documentId="13_ncr:1_{EC215A14-A98F-42F7-AC78-D064D6F40FAA}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
     <workbookView windowHeight="12456" windowWidth="23256" xWindow="-108" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-108"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>P1001</t>
   </si>
@@ -52,12 +52,6 @@
     <t>A001</t>
   </si>
   <si>
-    <t>896ab1861ca94ada3f55516470a58a13</t>
-  </si>
-  <si>
-    <t>dd92ecffeb88486b5f62143eb23d42164b4512f9d57a6bbeb8f40e74f7d25f6e</t>
-  </si>
-  <si>
     <t>890eba8336601ea76c2dc0f5593201ba</t>
   </si>
   <si>
@@ -88,22 +82,34 @@
     <t>8aad139cbe3a9d8e01d9c8b0de3130b48e3871c90f320e724a2740c8ea3a7305</t>
   </si>
   <si>
-    <t>2fc4c518f72b0ad141dac3e5f35e06e2</t>
-  </si>
-  <si>
-    <t>7a5582ff977775a6afb82b31b5f20f563c88025129d0cc188a5b7dd6afb566d2</t>
-  </si>
-  <si>
-    <t>72fff9c9e914cba450935325b88a0a0f</t>
-  </si>
-  <si>
-    <t>87ecb123e9cb12f7e37d7a1e752e1b9eea4f25f95ce2db005912128d766a206f</t>
-  </si>
-  <si>
     <t>9e77801637aa3e26e81b828b2225b19f</t>
   </si>
   <si>
     <t>bfc2e49bf9b642e1a8466c96bae32b96877931ddba9e8d3c7fd6df36cdfc88fe</t>
+  </si>
+  <si>
+    <t>ea6697e927d5087d08b5218455deb794</t>
+  </si>
+  <si>
+    <t>a74c91fe1367f03956a8afb4bdd0c201982122e1cf3fdd09ea2445e8cccaf5a6</t>
+  </si>
+  <si>
+    <t>D999</t>
+  </si>
+  <si>
+    <t>e809a49832b33d35c47689286b1cfbaa</t>
+  </si>
+  <si>
+    <t>85da2685c4bb4f84dfcb126a3ca4bc958ab9c8c27b24c80485fb34731f64a71e</t>
+  </si>
+  <si>
+    <t>P999</t>
+  </si>
+  <si>
+    <t>f86bf1e8753ab0a04d292050e6841f0e</t>
+  </si>
+  <si>
+    <t>b2597e074e2ab8822cc65737403429b1f1fa8139313b0907e05c316816bba347</t>
   </si>
 </sst>
 </file>
@@ -475,7 +481,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD9"/>
+      <selection activeCell="A9" sqref="A9:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -499,10 +505,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C2" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -510,10 +516,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -521,10 +527,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -532,10 +538,10 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -543,10 +549,10 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -554,10 +560,10 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>